<commit_message>
added L knots to image with magnifying glass
</commit_message>
<xml_diff>
--- a/assignment_01c/code_prototype.xlsx
+++ b/assignment_01c/code_prototype.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ripleycleghorn/Desktop/Masters/Major Studio 1/msdv-major-studio/assignment_01c/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7D3071AE-9CEE-CB4A-96BD-B45E0458F4C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D162CDFE-F68A-C845-B93A-6E354F18FB5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Heading" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pendant Detail'!$A$6:$I$185</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Pendant Detail'!$1:$6</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -557,7 +557,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1008,7 +1008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:A37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1188,11 +1188,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K549"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="183" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="183" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109:D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3766,7 +3766,7 @@
       <c r="B101" s="5">
         <v>48</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="9" t="s">
         <v>88</v>
       </c>
       <c r="E101" t="s">
@@ -3795,7 +3795,7 @@
       <c r="C102" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="9" t="s">
         <v>86</v>
       </c>
       <c r="E102" t="s">
@@ -3821,7 +3821,7 @@
       <c r="B103" s="5">
         <v>49</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="9" t="s">
         <v>89</v>
       </c>
       <c r="E103" t="s">
@@ -3850,7 +3850,7 @@
       <c r="C104" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="9" t="s">
         <v>90</v>
       </c>
       <c r="E104" t="s">
@@ -3873,7 +3873,7 @@
       <c r="B105" s="5">
         <v>50</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="9" t="s">
         <v>86</v>
       </c>
       <c r="E105" t="s">
@@ -3899,7 +3899,7 @@
       <c r="B106" s="5">
         <v>51</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="9" t="s">
         <v>100</v>
       </c>
       <c r="E106" t="s">
@@ -3925,7 +3925,7 @@
       <c r="B107" s="5">
         <v>52</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="9" t="s">
         <v>86</v>
       </c>
       <c r="E107" t="s">
@@ -3951,7 +3951,7 @@
       <c r="B108" s="5">
         <v>53</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="9" t="s">
         <v>100</v>
       </c>
       <c r="E108" t="s">
@@ -3977,7 +3977,7 @@
       <c r="B109" s="5">
         <v>54</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="9" t="s">
         <v>89</v>
       </c>
       <c r="E109" t="s">
@@ -4006,7 +4006,7 @@
       <c r="C110" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="9" t="s">
         <v>84</v>
       </c>
       <c r="E110" t="s">
@@ -5975,7 +5975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>